<commit_message>
Images added to menu
Images added and images added to data for menu
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\user\Documents\Mphasis\FoodDelivery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653C7B45-875F-4B54-9830-494F246700F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30262AA5-E8EC-4059-9046-3E72CC457E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{803F6772-99E4-4DDE-909D-048EFCFA1D68}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>UserID</t>
   </si>
@@ -196,6 +196,54 @@
   </si>
   <si>
     <t>A Dessert of sponge cake soaked in a mixture of condenced milk, evaporated milk, and cream</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>./foodImages/Spaghetti.jpg</t>
+  </si>
+  <si>
+    <t>./foodImages/PorkFriedRice.jpg</t>
+  </si>
+  <si>
+    <t>./foodImages/NachoCarbon.jpg</t>
+  </si>
+  <si>
+    <t>./foodImages/ChickenChimichangas.jpeg</t>
+  </si>
+  <si>
+    <t>./foodImages/GenralTsoChicken.jpg</t>
+  </si>
+  <si>
+    <t>./foodImages/Tiramisu.jpg</t>
+  </si>
+  <si>
+    <t>./foodImages/Lasagne.jpg</t>
+  </si>
+  <si>
+    <t>./foodImages/HunanShrimp.jpg</t>
+  </si>
+  <si>
+    <t>./foodImages/PolloAsado.jpg</t>
+  </si>
+  <si>
+    <t>./foodImages/ChickenTikkaMasala.jpg</t>
+  </si>
+  <si>
+    <t>./foodImages/Samosas.jpg</t>
+  </si>
+  <si>
+    <t>./foodImages/TresLeches.jpg</t>
+  </si>
+  <si>
+    <t>./foodImages/GoatVindaloo.jpg</t>
+  </si>
+  <si>
+    <t>./foodImages/Calamari.jpg</t>
+  </si>
+  <si>
+    <t>./foodImages/RasMalai.jpg</t>
   </si>
 </sst>
 </file>
@@ -260,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -283,6 +331,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,11 +649,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BDFF2A7-C2FB-40F8-BDB3-C1847EC9C624}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -613,10 +664,11 @@
     <col min="4" max="4" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.7109375" style="6" customWidth="1"/>
     <col min="6" max="6" width="6.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="43.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -635,11 +687,14 @@
       <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -658,11 +713,14 @@
       <c r="F2" s="11">
         <v>0.42</v>
       </c>
-      <c r="G2" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="G2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -681,11 +739,14 @@
       <c r="F3" s="11">
         <v>0.18</v>
       </c>
-      <c r="G3" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.2">
+      <c r="G3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -704,11 +765,14 @@
       <c r="F4" s="11">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G4" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -727,11 +791,14 @@
       <c r="F5" s="11">
         <v>1</v>
       </c>
-      <c r="G5" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="G5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -750,11 +817,14 @@
       <c r="F6" s="11">
         <v>1</v>
       </c>
-      <c r="G6" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -773,11 +843,14 @@
       <c r="F7" s="11">
         <v>0.52</v>
       </c>
-      <c r="G7" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="G7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -796,11 +869,14 @@
       <c r="F8" s="11">
         <v>0.73</v>
       </c>
-      <c r="G8" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="G8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -819,11 +895,14 @@
       <c r="F9" s="11">
         <v>1</v>
       </c>
-      <c r="G9" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.2">
+      <c r="G9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -842,11 +921,14 @@
       <c r="F10" s="11">
         <v>0.33</v>
       </c>
-      <c r="G10" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="G10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -865,11 +947,14 @@
       <c r="F11" s="11">
         <v>1</v>
       </c>
-      <c r="G11" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.2">
+      <c r="G11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -888,11 +973,14 @@
       <c r="F12" s="11">
         <v>1</v>
       </c>
-      <c r="G12" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="G12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -911,11 +999,14 @@
       <c r="F13" s="11">
         <v>0.81</v>
       </c>
-      <c r="G13" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="G13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -934,11 +1025,14 @@
       <c r="F14" s="11">
         <v>1</v>
       </c>
-      <c r="G14" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="G14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -957,11 +1051,14 @@
       <c r="F15" s="11">
         <v>0.67</v>
       </c>
-      <c r="G15" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.2">
+      <c r="G15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -980,7 +1077,10 @@
       <c r="F16" s="11">
         <v>1</v>
       </c>
-      <c r="G16" s="1" t="b">
+      <c r="G16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="1" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>